<commit_message>
moved fuzzy string match function to pyBlitz
</commit_message>
<xml_diff>
--- a/data/teamrankings.xlsx
+++ b/data/teamrankings.xlsx
@@ -2158,8 +2158,10 @@
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>